<commit_message>
modified:   Input/Specific Examer.xlsx 	modified:   __pycache__/class_def.cpython-311.pyc 	modified:   class_def.py 	modified:   main.ipynb 	modified:   try.ipynb 	new file:   "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
	modified:   main.ipynb
	modified:   main.py
	modified:   "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/Input/Specific Examer.xlsx
+++ b/Input/Specific Examer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5EBF09-BF5F-44A3-BB5B-C2F04418DC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC17AB0-453C-4E85-93FE-4CA983BF7587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tunayoshi</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{1E71CA32-AA06-4141-BBAD-BFB4A6127919}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>格式
+任教年級: 老師</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{FE882A7A-E6A0-44E3-9944-8C039C0EC312}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>格式
+老師: 時數比例</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>English Speaking
 主考官</t>
@@ -163,13 +203,40 @@
   </si>
   <si>
     <t>TSYE</t>
+  </si>
+  <si>
+    <t>特殊時數</t>
+  </si>
+  <si>
+    <t>CLC: 0.25</t>
+  </si>
+  <si>
+    <t>NSW: 0.25</t>
+  </si>
+  <si>
+    <t>OCW: 0.25</t>
+  </si>
+  <si>
+    <t>HLY: 0.5</t>
+  </si>
+  <si>
+    <t>TSW: 0</t>
+  </si>
+  <si>
+    <t>NYK: 0</t>
+  </si>
+  <si>
+    <t>FCH: 0</t>
+  </si>
+  <si>
+    <t>LSC: 0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +251,13 @@
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -351,7 +425,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -633,21 +707,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="11" width="16.6640625" customWidth="1"/>
+    <col min="4" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -673,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>12</v>
@@ -681,13 +755,16 @@
       <c r="K1" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -708,16 +785,19 @@
         <v>31</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -740,13 +820,16 @@
       <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>14</v>
@@ -767,13 +850,16 @@
       <c r="H4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>15</v>
@@ -790,13 +876,16 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -813,13 +902,16 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -836,13 +928,16 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -859,11 +954,14 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K8" s="4"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -880,11 +978,14 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K9" s="4"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>18</v>
@@ -899,9 +1000,10 @@
       <c r="H10" s="4"/>
       <c r="I10" s="2"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K10" s="4"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>19</v>
@@ -916,9 +1018,10 @@
       <c r="H11" s="4"/>
       <c r="I11" s="2"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K11" s="4"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>20</v>
@@ -933,9 +1036,10 @@
       <c r="H12" s="4"/>
       <c r="I12" s="2"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K12" s="4"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>21</v>
@@ -950,11 +1054,14 @@
       <c r="H13" s="4"/>
       <c r="I13" s="2"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K13" s="4"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -963,9 +1070,10 @@
       <c r="H14" s="4"/>
       <c r="I14" s="2"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K14" s="4"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -976,9 +1084,10 @@
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K15" s="4"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -989,9 +1098,10 @@
       <c r="H16" s="4"/>
       <c r="I16" s="2"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K16" s="4"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1002,9 +1112,10 @@
       <c r="H17" s="4"/>
       <c r="I17" s="2"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K17" s="4"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1015,9 +1126,10 @@
       <c r="H18" s="4"/>
       <c r="I18" s="2"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K18" s="4"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1028,9 +1140,10 @@
       <c r="H19" s="4"/>
       <c r="I19" s="2"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="K19" s="4"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1041,9 +1154,10 @@
       <c r="H20" s="5"/>
       <c r="I20" s="3"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K20" s="5"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1055,7 +1169,7 @@
       <c r="I21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1067,7 +1181,7 @@
       <c r="I22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1079,7 +1193,7 @@
       <c r="I23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1091,7 +1205,7 @@
       <c r="I24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1103,7 +1217,7 @@
       <c r="I25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1115,7 +1229,7 @@
       <c r="I26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1127,7 +1241,7 @@
       <c r="I27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1139,7 +1253,7 @@
       <c r="I28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1151,7 +1265,7 @@
       <c r="I29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1163,7 +1277,7 @@
       <c r="I30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1175,7 +1289,7 @@
       <c r="I31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1286,5 +1400,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>